<commit_message>
updated PR scenario 3 and 4
</commit_message>
<xml_diff>
--- a/testconfigs/testdata/testdata.xlsx
+++ b/testconfigs/testdata/testdata.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Social Registry Sanity UI Automation\edrmc-portal-forms-automated\testconfigs\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB947FF-0444-4839-8B13-DE81DDB10681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F5087D-30C9-4708-A974-95610E8D375F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="6045" activeTab="3" xr2:uid="{A4B71DF1-AF07-4093-B6CF-CBEFC387B227}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="6045" firstSheet="1" activeTab="5" xr2:uid="{A4B71DF1-AF07-4093-B6CF-CBEFC387B227}"/>
   </bookViews>
   <sheets>
     <sheet name="resetPassword" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
     <sheet name="scenarioPR1" sheetId="3" r:id="rId3"/>
     <sheet name="scenarioPR2" sheetId="4" r:id="rId4"/>
+    <sheet name="scenarioPR3" sheetId="5" r:id="rId5"/>
+    <sheet name="scenarioPR4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="82">
   <si>
     <t>email</t>
   </si>
@@ -241,6 +243,39 @@
   </si>
   <si>
     <t>+251912345676</t>
+  </si>
+  <si>
+    <t>123456789034</t>
+  </si>
+  <si>
+    <t>+251912345674</t>
+  </si>
+  <si>
+    <t>+251912345673</t>
+  </si>
+  <si>
+    <t>auto test user3</t>
+  </si>
+  <si>
+    <t>testuser3@gmail.com</t>
+  </si>
+  <si>
+    <t>mem3@gmail.com</t>
+  </si>
+  <si>
+    <t>123456654321</t>
+  </si>
+  <si>
+    <t>auto test user4</t>
+  </si>
+  <si>
+    <t>testuser4@gmail.com</t>
+  </si>
+  <si>
+    <t>Auto Member4</t>
+  </si>
+  <si>
+    <t>mem4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -989,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C570C82F-AFA3-4CB6-9891-B44A989C7EB4}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,4 +1323,612 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4C7F5A-F901-41BA-A1E1-C10A4C381C89}">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{84409599-1D06-4E8F-B9FB-FCA3BDF93701}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{7F1A4BAE-5D78-4181-B0D6-9BAEFAB3B9C7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8A1B98-645D-4287-9CFD-7312B6327106}">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C150499-3E2C-442D-952A-C7BBBFCEA5CF}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{6E2DCD86-504C-4B15-9FF1-6AE8FC0931AA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>